<commit_message>
add task spliter analyze per kr per person
</commit_message>
<xml_diff>
--- a/assets/excel/team tasks spreadsheet.xlsx
+++ b/assets/excel/team tasks spreadsheet.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\OKR_analyze\assets\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA222AA-E474-4683-BB37-6F3FD04FC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>date</t>
   </si>
@@ -131,6 +122,9 @@
     <t>1- Scraping Bazar comments 2-'Generative AI Course with a Focus on Large Language Models' at Hamrah Academy</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Monday</t>
   </si>
   <si>
@@ -158,7 +152,8 @@
     <t xml:space="preserve">1- جلسه با آقای اژدری 2-نوشتن اولین کد پروژه و دریافت اولین خروجی از LLM </t>
   </si>
   <si>
-    <t>1- Scraping Bazar comments</t>
+    <t>1- Scraping Bazar comments
+2- Meeting With Mr Azhdari</t>
   </si>
   <si>
     <t>1- جلاسه معاونت
@@ -221,6 +216,10 @@
 2- develop first ui version to enter parameter manualy</t>
   </si>
   <si>
+    <t>1-بررسی و اصلاح برخی دسترسی ها در ریپورت سرو
+2-اصلاح etl مرتبط با اینترکانکت</t>
+  </si>
+  <si>
     <t xml:space="preserve">1- ساخت مینی گزارش بودجه به همراه حسین قربانی
 2- بررسی شاخص آرپو و گرفتن تایید از اردستانی جهت اتوماسیون 
 3- ساخت SP برای دریافت اطلاعات آرپو و ساخت داشبورد </t>
@@ -245,28 +244,139 @@
 2- بررسی آخرین وضعیت ورود عملکرد شاخص عهای خودکار شده و پیگیری برای دسترسی سریعتر به داده های اولیه</t>
   </si>
   <si>
+    <t xml:space="preserve">
+1- بررسی دیتای ارسالی شاخص های آموزش در منابع انسانی به منظور اتوماسیون - جلسه با مسئول شاخص - محاسبات اولیه عدد فصل چهارم شاخص
+2- کار روی مدل پیش بینی زمان تایید مسئولین گام های پروژه در راستای افزایش دقت</t>
+  </si>
+  <si>
+    <t>1-اکسل یوزر ها در ریپورت سرور
+2- پیگیری تیکت</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- ساخت ادامه گزارش قزبانی
+2- بررسی درآمد و مغایرت های آن 
+3- تکمیل اصلاحات گزارش Market Share
+</t>
+  </si>
+  <si>
     <t>1- writing queries in sql for province KPIs(MNP).          2- checking CRA data</t>
   </si>
   <si>
-    <t xml:space="preserve">1-نصب پایتون بر روی سرور لینوکسی برای تست پیش نیاز اجرای LLM 2-بررسی برنامه خواندن ایمیل و انتقال به سرور                                                                                            </t>
+    <t>1-نصب پایتون بر روی سرور لینوکسی برای تست پیش نیاز اجرای LLM 2-بررسی برنامه خواندن ایمیل و انتقال به سرور 3-تغییر و بهبود کد ارزیابی okr  3-ایجاد نسخه اولیه توضیحات هر KR تیم با هوش مصنوعی و اصلاح KR های مرتبط با خود و ارسال برای تایید نهایی آقای رضازاده</t>
   </si>
   <si>
     <t>1-Development of OKR UI: okr status page (deliverables and risks)</t>
+  </si>
+  <si>
+    <t>1- پیگیری علت عدم اپدیت شاخص های خودکار
+2- پیگیری تیکت اتصال 161 به FTP فراز
+3- پیگیری تیکت اتصال 82 به FTP فراز
+4- پیگیری تیکت انتقال سرور 146 به زون CT
+5- پیگیری نصب GPU بر روی سرور جدید 50 و ایجاد اکانت بر روی سرورهای جدید
+6- بررسی هفتگی برنامه OKR تیم با آقای یوسفی
+7- تدوین برنامه OKR تیم برای فصل اول 
+8- نوشتن شرح نتایج کلیدی OKR تیم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- دریافت دیتای فصل جدید 6 شاخص اتومات شده خرید و آپدیت و محاسبات برای فصل چهارم و صحت سنجی نتایج
+2- آپدیت و انجام اصلاحات شاخص های اتومات شده خدمات مشتریان با در نظر گرفتن اصلاحات مشخص معاونت خدمات مشتریان
+3- چک و آپدیت شاخص های اتومات FMRA و اصلاح طبق درخواست مسئول حوزه </t>
+  </si>
+  <si>
+    <t>1-ایمپورت شیت دوم دیتای فراد
+2-اصلاح پروسیجر داشبورد درآمد
+3-اصلاج کویری شاخص 51456 برای درآمد کل</t>
+  </si>
+  <si>
+    <t>1- بررسی دیتای درآمد و مقایسه آن با اعداد شاخصها و فایل دریافتی از اردستانی
+2- ساخت گزارش Arpu</t>
+  </si>
+  <si>
+    <t>checking  revenue KPIs</t>
+  </si>
+  <si>
+    <t>1-چک کردن برنامه دریافت ایمیل سازمانی و ارسال فایل ها به سرور 2-بررسی هفتگی okr تیم با آقای رضازاده و یوسفی 3-اتمام کد افزودن توضیحات KR ها به پرامپت ارزیابی OKR</t>
+  </si>
+  <si>
+    <t>1- Scraping Bazar comments
+2- Scraping Google Play comments</t>
+  </si>
+  <si>
+    <t>1- پیگیری تیکت اتصال 161 به FTP فراز
+2- پیگیری تیکت اتصال 82 به FTP فراز
+3- پیگیری تیکت انتقال سرور 146 به زون CT
+4- پیگیری ارسال داده های درآمدی روزانه
+5- پیگیری رفع مشکل حذف اسکریپت شاخص های خودکار شده
+6- ارایه داشبوردهای تهیه شده به مهمان آقای ازدری
+7- نوشتن شرح نتایج کلیدی OKR تیم</t>
+  </si>
+  <si>
+    <t>1-بررسی ایراد دیتای اینترکانکت
+2- بررسی دیتای بالک
+3-ساخت پروسیجر ذخیره کویری های اتوماسیون در یک جدول
+4- ایجاد پکیج و جاب برای انتقال کویری اتوماسیون شاخص ها به دیتابیس استیج
+5- اصلاح کویری شاخص مرتبط با در امد- کد شاخص 51456</t>
+  </si>
+  <si>
+    <t>1- تکمیل گزارش Arpu
+2- نهایی سازی تم داشبوردها 
+3- آموزش BI به آرمان و نحوه دسترسی به دیتاها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-event entry                2- checking revenue KPIs </t>
+  </si>
+  <si>
+    <t>1- بررسی برنامه دریافت ایمیل سازمانی و نصب پکیج های پایتون روی سیستم BIfetch و نوشتن اسکریپت برای اجرای کد از طریق پایتون به صورت خودکار 2-نوشتن پرامپت و کد برای دریافت تسک های روزانه افراد و ترجمه و همزبان سازی و جداکردن تسک های روزانه و آماده سازی برای ذخیره در دیتابیس 3-نوشتن اسکریپت برای باز کردن outlook و سپس اجرای برنامه خواندن ایمیل های سازمانی برای جلوگیری از درخواست پسورد</t>
+  </si>
+  <si>
+    <t>1-Development of OKR UI: task page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-کار بر روی داشبورد 
+Data Effective Price
+2-جستجوی نمونه داشبورد های
+3-جلسه با آقای زاهدی جهت آموزش و
+آشنایی با سرورها و نحوه دسترسی
+</t>
+  </si>
+  <si>
+    <t>1- نوشتن شرح نتایج کلیدی OKR تیم
+2- بررسی گزارشات تحلیلی در خصوص اقتصاد دیجیتال</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- بررسی دیتاهای   B2B
+2- بررسی Pipeline  داده های درآمدی جهت سحت سنجی آن ها 
+3- آموزش </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- inbound roaming automation: create new sp and x.                     2- checking VDI environment for future use cases </t>
+  </si>
+  <si>
+    <t>1-شرکت در وبینار استراتژی های هوش مصنوعی در شکرت های فناوری برتر دنیا 2-تکمیل کد جدا کردن تسک های روزانه و ذخیره در دیتابیس و گیت هاب 3-نوشتن کد جدید برای جمع آوری ایمیل های سازمانی و اجرا در سیستم bifetch 4-گرفتن سمپل دیتا از اسفند 1403 تا 15 اردیبهشت 1402 برای ایونت های خروجی سامانه تحلیل ایونت</t>
+  </si>
+  <si>
+    <t>1-Development of OKR UI: Connecting the Frontend and Backend
+2- Scrape Tweets from X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -277,61 +387,60 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+  <cellXfs count="10">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -521,32 +630,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A8:XFD16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col customWidth="1" min="6" max="6" width="23.88"/>
+    <col customWidth="1" min="7" max="7" width="13.0"/>
+    <col customWidth="1" min="9" max="9" width="12.63"/>
+    <col customWidth="1" min="10" max="10" width="15.63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,9 +684,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="344.25" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="1">
-        <v>14040206</v>
+        <v>1.4040206E7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -608,9 +714,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="267.75" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="1">
-        <v>14040207</v>
+        <v>1.4040207E7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
@@ -634,160 +740,230 @@
       <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" ht="95.25" customHeight="1">
       <c r="A4" s="1">
-        <v>14040208</v>
+        <v>1.4040208E7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="331.5" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1">
-        <v>14040209</v>
+        <v>1.4040209E7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="331.5" x14ac:dyDescent="0.2">
+      <c r="J5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1">
-        <v>14040210</v>
+        <v>1.404021E7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="F6" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="1">
-        <v>14040213</v>
+        <v>1.4040213E7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="G7" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-    </row>
-    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
+        <v>57</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>1.4040214E7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>1.4040215E7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1.4040216E7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>1.4040217E7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -797,9 +973,13 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>1.404022E7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -809,9 +989,13 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>1.4040221E7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -821,9 +1005,13 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>1.4040222E7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -833,9 +1021,13 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>1.4040223E7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -845,9 +1037,13 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>1.4040224E7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -858,6 +1054,6 @@
       <c r="J16" s="3"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>